<commit_message>
added exam dates and times to calendar
</commit_message>
<xml_diff>
--- a/2026-ph102-spring.xlsx
+++ b/2026-ph102-spring.xlsx
@@ -176,7 +176,10 @@
     <t xml:space="preserve">** Study Day **</t>
   </si>
   <si>
-    <t xml:space="preserve">** FINAL EXAMS **</t>
+    <t xml:space="preserve">** FINAL EXAMS **
+Section 01 → Tuesday, April 28th at 1pm
+Section 02 → Wednesday, April 29th at 8am
+Section 03 → Monday, April 27th at 8am</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -805,8 +808,8 @@
   </sheetPr>
   <dimension ref="A2:AMI109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M79" activeCellId="0" sqref="M79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F104" activeCellId="0" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1314,7 +1317,7 @@
       <c r="AMI27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="22" t="n">
         <f aca="false">IF(B27="",B26+IF(OR(WEEKDAY(B26)=2,WEEKDAY(B26)=4),2,3),"")</f>
         <v>46057</v>
@@ -1785,7 +1788,7 @@
       <c r="AMI51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="22" t="n">
         <f aca="false">IF(B51="",B50+IF(OR(WEEKDAY(B50)=2,WEEKDAY(B50)=4),2,3),"")</f>
         <v>46085</v>
@@ -2299,7 +2302,7 @@
       <c r="AMI79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="15" t="n">
         <f aca="false">IF(B79="",B78+IF(OR(WEEKDAY(B78)=2,WEEKDAY(B78)=4),2,3),"")</f>
         <v>46118</v>
@@ -2757,7 +2760,7 @@
       <c r="AMI103" s="2"/>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0"/>
+      <c r="A104" s="29"/>
       <c r="B104" s="15" t="n">
         <f aca="false">IF(B103="",B102+IF(OR(WEEKDAY(B102)=2,WEEKDAY(B102)=4),2,3),"")</f>
         <v>46146</v>

</xml_diff>